<commit_message>
BOM - Assembled mixer-MAC-24+
</commit_message>
<xml_diff>
--- a/bom/filter-misc.xlsx
+++ b/bom/filter-misc.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emastro\Documents\OreSat\GitHub\oresat-c3-rf\bom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5618E3D5-01C8-4C45-838D-9542431CF801}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3FBE9D8-E206-4295-8AA8-B9F799D419A6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3280" yWindow="1730" windowWidth="24000" windowHeight="12760" tabRatio="790" xr2:uid="{43A8C8E3-6B11-4AFF-A143-79A3AF0034F8}"/>
+    <workbookView xWindow="1140" yWindow="1140" windowWidth="25580" windowHeight="15470" tabRatio="790" activeTab="3" xr2:uid="{43A8C8E3-6B11-4AFF-A143-79A3AF0034F8}"/>
   </bookViews>
   <sheets>
     <sheet name="bpf-IF-SAW-856930" sheetId="6" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="86">
   <si>
     <t>Notes</t>
   </si>
@@ -178,9 +178,6 @@
     <t>AT1, AT2, AT3</t>
   </si>
   <si>
-    <t>Z1, Z2, Z3, AT1, AT2, AT3</t>
-  </si>
-  <si>
     <t>Susumu</t>
   </si>
   <si>
@@ -287,6 +284,27 @@
   </si>
   <si>
     <t>Filter, thin-film 0805, 1220 - 1420 MHz</t>
+  </si>
+  <si>
+    <t>USED</t>
+  </si>
+  <si>
+    <t>Z1, Z2, Z3</t>
+  </si>
+  <si>
+    <t>RMCF0603ZT0R00‎</t>
+  </si>
+  <si>
+    <t>R - 0603, 0, jumper</t>
+  </si>
+  <si>
+    <t>RMCF0603ZT0R00CT-ND‎</t>
+  </si>
+  <si>
+    <t>Assembled 1x board w/ all 0 ohm</t>
+  </si>
+  <si>
+    <t>DNP</t>
   </si>
 </sst>
 </file>
@@ -309,7 +327,7 @@
       <name val="Sans"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -319,6 +337,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -344,7 +368,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -387,6 +411,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -704,8 +731,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7511E1D-1F43-4E9A-A428-C582B74E68D7}">
   <dimension ref="A1:L18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5"/>
@@ -742,7 +769,7 @@
     </row>
     <row r="2" spans="1:12" ht="13">
       <c r="A2" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="4"/>
@@ -848,7 +875,7 @@
         <v>2</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C8" t="s">
         <v>10</v>
@@ -889,25 +916,25 @@
         <v>9</v>
       </c>
       <c r="E9" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="F9" s="17" t="s">
         <v>73</v>
       </c>
-      <c r="F9" s="17" t="s">
+      <c r="G9" s="17" t="s">
         <v>74</v>
       </c>
-      <c r="G9" s="17" t="s">
+      <c r="H9" s="17" t="s">
         <v>75</v>
       </c>
-      <c r="H9" s="17" t="s">
+      <c r="I9" s="17" t="s">
         <v>76</v>
-      </c>
-      <c r="I9" s="17" t="s">
-        <v>77</v>
       </c>
       <c r="J9" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K9" s="17" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -978,7 +1005,7 @@
   <dimension ref="A1:L18"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5"/>
@@ -1015,7 +1042,7 @@
     </row>
     <row r="2" spans="1:12" ht="13">
       <c r="A2" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="4"/>
@@ -1121,7 +1148,7 @@
         <v>2</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C8" t="s">
         <v>10</v>
@@ -1152,8 +1179,8 @@
       <c r="A9" s="1">
         <v>1</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>50</v>
+      <c r="B9" s="9" t="s">
+        <v>41</v>
       </c>
       <c r="C9" t="s">
         <v>37</v>
@@ -1162,19 +1189,19 @@
         <v>9</v>
       </c>
       <c r="E9" s="17" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F9" s="17" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G9" s="17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H9" s="17" t="s">
         <v>5</v>
       </c>
       <c r="I9" s="17" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J9" s="1" t="s">
         <v>4</v>
@@ -1248,7 +1275,7 @@
   <dimension ref="A1:L18"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5"/>
@@ -1285,7 +1312,7 @@
     </row>
     <row r="2" spans="1:12" ht="13">
       <c r="A2" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="4"/>
@@ -1391,7 +1418,7 @@
         <v>3</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C8" t="s">
         <v>36</v>
@@ -1422,8 +1449,8 @@
       <c r="A9" s="1">
         <v>1</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>50</v>
+      <c r="B9" s="9" t="s">
+        <v>41</v>
       </c>
       <c r="C9" t="s">
         <v>37</v>
@@ -1432,19 +1459,19 @@
         <v>9</v>
       </c>
       <c r="E9" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="F9" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="F9" s="17" t="s">
+      <c r="G9" s="17" t="s">
         <v>65</v>
-      </c>
-      <c r="G9" s="17" t="s">
-        <v>66</v>
       </c>
       <c r="H9" s="17" t="s">
         <v>5</v>
       </c>
       <c r="I9" s="17" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J9" s="1" t="s">
         <v>4</v>
@@ -1515,10 +1542,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78247F15-604B-4815-817D-5809FD1D0A84}">
-  <dimension ref="A1:L23"/>
+  <dimension ref="A1:L24"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B42" sqref="B42"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5"/>
@@ -1655,8 +1682,8 @@
       <c r="A8" s="1">
         <v>3</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>50</v>
+      <c r="B8" s="19" t="s">
+        <v>79</v>
       </c>
       <c r="C8" t="s">
         <v>36</v>
@@ -1687,8 +1714,8 @@
       <c r="A9" s="1">
         <v>1</v>
       </c>
-      <c r="B9" s="9" t="s">
-        <v>41</v>
+      <c r="B9" s="19" t="s">
+        <v>79</v>
       </c>
       <c r="C9" t="s">
         <v>37</v>
@@ -1716,148 +1743,192 @@
       <c r="A10" s="1">
         <v>4</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>50</v>
+      <c r="B10" s="9" t="s">
+        <v>41</v>
       </c>
       <c r="C10" t="s">
         <v>42</v>
       </c>
+      <c r="D10" s="1" t="s">
+        <v>85</v>
+      </c>
       <c r="E10" s="11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F10" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G10" s="11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H10" s="14" t="s">
         <v>5</v>
       </c>
       <c r="I10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:12">
       <c r="A11" s="1">
         <v>2</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>50</v>
+      <c r="B11" s="9" t="s">
+        <v>41</v>
       </c>
       <c r="C11" t="s">
         <v>42</v>
       </c>
+      <c r="D11" s="1" t="s">
+        <v>85</v>
+      </c>
       <c r="E11" s="11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F11" s="11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G11" s="11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H11" s="14" t="s">
         <v>5</v>
       </c>
       <c r="I11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:12">
       <c r="A12" s="1">
         <v>2</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>50</v>
+      <c r="B12" s="9" t="s">
+        <v>41</v>
       </c>
       <c r="C12" t="s">
         <v>42</v>
       </c>
+      <c r="D12" s="1" t="s">
+        <v>85</v>
+      </c>
       <c r="E12" s="11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F12" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G12" s="11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H12" s="14" t="s">
         <v>5</v>
       </c>
       <c r="I12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:12">
       <c r="A13" s="1">
         <v>2</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>50</v>
+      <c r="B13" s="9" t="s">
+        <v>41</v>
       </c>
       <c r="C13" t="s">
         <v>42</v>
       </c>
+      <c r="D13" s="1" t="s">
+        <v>85</v>
+      </c>
       <c r="E13" s="11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F13" s="11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G13" s="11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H13" s="14" t="s">
         <v>5</v>
       </c>
       <c r="I13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:12">
       <c r="A14" s="1">
-        <v>6</v>
-      </c>
-      <c r="B14" s="9" t="s">
-        <v>41</v>
+        <v>3</v>
+      </c>
+      <c r="B14" s="19" t="s">
+        <v>79</v>
       </c>
       <c r="C14" t="s">
-        <v>43</v>
+        <v>80</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E14" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="F14" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="F14" s="11" t="s">
+      <c r="G14" s="11" t="s">
         <v>47</v>
-      </c>
-      <c r="G14" s="11" t="s">
-        <v>48</v>
       </c>
       <c r="H14" s="15" t="s">
         <v>5</v>
       </c>
       <c r="I14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J14" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
+      <c r="A15" s="1">
+        <v>3</v>
+      </c>
+      <c r="B15" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="C15" t="s">
+        <v>42</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15" s="11" t="s">
         <v>45</v>
+      </c>
+      <c r="F15" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="G15" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="H15" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="I15" t="s">
+        <v>83</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="17" spans="1:12">
@@ -1900,6 +1971,14 @@
       </c>
       <c r="C23" t="s">
         <v>31</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12">
+      <c r="B24" s="2">
+        <v>43738</v>
+      </c>
+      <c r="C24" t="s">
+        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>